<commit_message>
#172 Tag ColsFit isn't working for worksheet column
</commit_message>
<xml_diff>
--- a/tests/Templates/5_options.xlsx
+++ b/tests/Templates/5_options.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="120" windowWidth="28635" windowHeight="12585"/>
@@ -11,12 +11,12 @@
     <sheet name="Лист2" sheetId="2" r:id="rId2"/>
     <sheet name="Лист3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
   <si>
     <t>&lt;&lt;OnlyValues&gt;&gt;</t>
   </si>
@@ -25,6 +25,21 @@
   </si>
   <si>
     <t>&amp;=10&lt;&lt;OnlyValues&gt;&gt;</t>
+  </si>
+  <si>
+    <t>asd</t>
+  </si>
+  <si>
+    <t>dsadasdasdasdasd</t>
+  </si>
+  <si>
+    <t>&lt;&lt;ColsFit&gt;&gt;</t>
+  </si>
+  <si>
+    <t>dsads</t>
+  </si>
+  <si>
+    <t>sdsasa</t>
   </si>
 </sst>
 </file>
@@ -361,10 +376,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:D11"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B59" sqref="B59"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="10.5"/>
@@ -373,24 +388,44 @@
     <col min="4" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:4">
+    <row r="1" spans="1:5">
+      <c r="D1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:5">
       <c r="B3" s="1" t="str">
         <f ca="1">CONCATENATE("Begin at ",TEXT(TODAY()-7,"dd.MM.yyyy"))</f>
         <v>Begin at dd.MM.yyyy</v>
       </c>
-    </row>
-    <row r="4" spans="1:4">
+      <c r="D3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
       <c r="B4" s="1"/>
-    </row>
-    <row r="6" spans="1:4">
+      <c r="D4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
       <c r="B6" s="1"/>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:5">
       <c r="D11" s="2"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
#172 Tag ColsFit isn't working for worksheet column (#176)
</commit_message>
<xml_diff>
--- a/tests/Templates/5_options.xlsx
+++ b/tests/Templates/5_options.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="120" windowWidth="28635" windowHeight="12585"/>
@@ -11,12 +11,12 @@
     <sheet name="Лист2" sheetId="2" r:id="rId2"/>
     <sheet name="Лист3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
   <si>
     <t>&lt;&lt;OnlyValues&gt;&gt;</t>
   </si>
@@ -25,6 +25,21 @@
   </si>
   <si>
     <t>&amp;=10&lt;&lt;OnlyValues&gt;&gt;</t>
+  </si>
+  <si>
+    <t>asd</t>
+  </si>
+  <si>
+    <t>dsadasdasdasdasd</t>
+  </si>
+  <si>
+    <t>&lt;&lt;ColsFit&gt;&gt;</t>
+  </si>
+  <si>
+    <t>dsads</t>
+  </si>
+  <si>
+    <t>sdsasa</t>
   </si>
 </sst>
 </file>
@@ -361,10 +376,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:D11"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B59" sqref="B59"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="10.5"/>
@@ -373,24 +388,44 @@
     <col min="4" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:4">
+    <row r="1" spans="1:5">
+      <c r="D1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:5">
       <c r="B3" s="1" t="str">
         <f ca="1">CONCATENATE("Begin at ",TEXT(TODAY()-7,"dd.MM.yyyy"))</f>
         <v>Begin at dd.MM.yyyy</v>
       </c>
-    </row>
-    <row r="4" spans="1:4">
+      <c r="D3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
       <c r="B4" s="1"/>
-    </row>
-    <row r="6" spans="1:4">
+      <c r="D4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
       <c r="B6" s="1"/>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:5">
       <c r="D11" s="2"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix test that started to fail after upgrading calc engine in ClosedXML;  make the test culture-independent
</commit_message>
<xml_diff>
--- a/tests/Templates/5_options.xlsx
+++ b/tests/Templates/5_options.xlsx
@@ -1,17 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20400"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\opensource\ClosedXML.Report\tests\Templates\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12F771B1-E0E4-44DF-8F50-ADC17E1795E5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="120" windowWidth="28635" windowHeight="12585"/>
+    <workbookView xWindow="120" yWindow="120" windowWidth="28632" windowHeight="12588" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
     <sheet name="Лист2" sheetId="2" r:id="rId2"/>
     <sheet name="Лист3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="191029"/>
 </workbook>
 </file>
 
@@ -45,11 +51,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yy\ h:mm;@"/>
   </numFmts>
-  <fonts count="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="8"/>
       <color theme="1"/>
@@ -88,6 +94,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -134,7 +148,7 @@
     </a:clrScheme>
     <a:fontScheme name="Стандартная">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -166,9 +180,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -200,6 +232,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Стандартная">
@@ -375,20 +425,18 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="10.5"/>
+  <sheetFormatPr defaultRowHeight="10.199999999999999" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D1" t="s">
         <v>5</v>
       </c>
@@ -396,15 +444,15 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B3" s="1" t="str">
-        <f ca="1">CONCATENATE("Begin at ",TEXT(TODAY()-7,"dd.MM.yyyy"))</f>
-        <v>Begin at dd.MM.yyyy</v>
+        <f>CONCATENATE("Begin at ","19.01.2023")</f>
+        <v>Begin at 19.01.2023</v>
       </c>
       <c r="D3" t="s">
         <v>3</v>
@@ -413,7 +461,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B4" s="1"/>
       <c r="D4" t="s">
         <v>6</v>
@@ -422,10 +470,10 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B6" s="1"/>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D11" s="2"/>
     </row>
   </sheetData>
@@ -435,16 +483,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="10.5"/>
+  <sheetFormatPr defaultRowHeight="10.199999999999999" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="2" spans="1:1">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -455,16 +503,16 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="10.5"/>
+  <sheetFormatPr defaultRowHeight="10.199999999999999" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="4" spans="2:2">
+    <row r="4" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>2</v>
       </c>

</xml_diff>

<commit_message>
Upgrade to ClosedXML 0.101 (#321)
* Upgrade to ClosedXML 0.101; target netstandard2.0 and netstandard2.1

* Fix test that started to fail after upgrading calc engine in ClosedXML;  make the test culture-independent
</commit_message>
<xml_diff>
--- a/tests/Templates/5_options.xlsx
+++ b/tests/Templates/5_options.xlsx
@@ -1,17 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20400"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\opensource\ClosedXML.Report\tests\Templates\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12F771B1-E0E4-44DF-8F50-ADC17E1795E5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="120" windowWidth="28635" windowHeight="12585"/>
+    <workbookView xWindow="120" yWindow="120" windowWidth="28632" windowHeight="12588" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
     <sheet name="Лист2" sheetId="2" r:id="rId2"/>
     <sheet name="Лист3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="191029"/>
 </workbook>
 </file>
 
@@ -45,11 +51,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yy\ h:mm;@"/>
   </numFmts>
-  <fonts count="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="8"/>
       <color theme="1"/>
@@ -88,6 +94,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -134,7 +148,7 @@
     </a:clrScheme>
     <a:fontScheme name="Стандартная">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -166,9 +180,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -200,6 +232,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Стандартная">
@@ -375,20 +425,18 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="10.5"/>
+  <sheetFormatPr defaultRowHeight="10.199999999999999" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D1" t="s">
         <v>5</v>
       </c>
@@ -396,15 +444,15 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B3" s="1" t="str">
-        <f ca="1">CONCATENATE("Begin at ",TEXT(TODAY()-7,"dd.MM.yyyy"))</f>
-        <v>Begin at dd.MM.yyyy</v>
+        <f>CONCATENATE("Begin at ","19.01.2023")</f>
+        <v>Begin at 19.01.2023</v>
       </c>
       <c r="D3" t="s">
         <v>3</v>
@@ -413,7 +461,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B4" s="1"/>
       <c r="D4" t="s">
         <v>6</v>
@@ -422,10 +470,10 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B6" s="1"/>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D11" s="2"/>
     </row>
   </sheetData>
@@ -435,16 +483,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="10.5"/>
+  <sheetFormatPr defaultRowHeight="10.199999999999999" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="2" spans="1:1">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -455,16 +503,16 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="10.5"/>
+  <sheetFormatPr defaultRowHeight="10.199999999999999" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="4" spans="2:2">
+    <row r="4" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>2</v>
       </c>

</xml_diff>